<commit_message>
BABA NDIAYE Tx d'inflation
</commit_message>
<xml_diff>
--- a/Indicateurs.xlsx
+++ b/Indicateurs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\TABLEAU_DE_BORD_CEP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BABA NDIAYE\Desktop\TABLEAU_DE_BORD_CEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="Annuelle" sheetId="1" r:id="rId1"/>
@@ -445,10 +445,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _C_F_A_-;\-* #,##0.00\ _C_F_A_-;_-* &quot;-&quot;??\ _C_F_A_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _C_F_A_-;\-* #,##0.00\ _C_F_A_-;_-* &quot;-&quot;??\ _C_F_A_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -856,12 +856,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -870,7 +870,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -925,7 +925,7 @@
     <xf numFmtId="1" fontId="14" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1031,18 +1031,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
@@ -1463,9 +1464,9 @@
   </sheetPr>
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -1989,6 +1990,9 @@
       </c>
       <c r="C8" s="88">
         <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D8" s="90">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -29456,13 +29460,13 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
+      <selection pane="bottomRight" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -31131,6 +31135,9 @@
       <c r="A91" s="52" t="s">
         <v>108</v>
       </c>
+      <c r="B91" s="17" t="s">
+        <v>118</v>
+      </c>
       <c r="C91" s="17" t="s">
         <v>118</v>
       </c>
@@ -31139,11 +31146,6 @@
       </c>
       <c r="E91" s="51"/>
       <c r="F91" s="15"/>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="B94" s="17" t="s">
-        <v>118</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B4 B10:B61 B63:B79 B81:B88 B92:B93 B95:B1048576">
@@ -31182,7 +31184,7 @@
   <conditionalFormatting sqref="C89:C91">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B89:B90 B94">
+  <conditionalFormatting sqref="B89:B91">
     <cfRule type="duplicateValues" dxfId="0" priority="25"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
BABA REMISE TX INF
</commit_message>
<xml_diff>
--- a/Indicateurs.xlsx
+++ b/Indicateurs.xlsx
@@ -1466,7 +1466,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -1991,9 +1991,7 @@
       <c r="C8" s="88">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="D8" s="90">
-        <v>2.5000000000000001E-2</v>
-      </c>
+      <c r="D8" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>